<commit_message>
Updated class-search for color model.
</commit_message>
<xml_diff>
--- a/class-search/BrowsingSimulation-ILSVRC2012.xlsx
+++ b/class-search/BrowsingSimulation-ILSVRC2012.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7848" windowHeight="4500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7848" windowHeight="4500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -133,6 +133,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1629,6 +1630,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1710,6 +1712,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>96</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>5</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2393,6 +2433,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.192</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.318</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.34100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.35599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.373</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.40400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.42399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.45300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.46100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.46800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.47899999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2500,6 +2600,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.219</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.253</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34499999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.36199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.377</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.38900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.44400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.44900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.45700000000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2847,38 +3007,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2931,6 +3059,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>Display 24</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t>, MLES depth 2</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3614,6 +3772,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.113</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.14799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.18099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.191</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.20799999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3721,6 +3939,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6999999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.115</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.13600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.16900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.17399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.17699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.184</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4068,38 +4346,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -4152,6 +4398,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>24</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>3</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -4835,6 +5119,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.127</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.155</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.186</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.19400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.21099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.217</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4942,6 +5286,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.107</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.13800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.157</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.186</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.20599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.21199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.214</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5289,38 +5693,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5373,6 +5745,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>24</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>5</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -6056,6 +6466,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>4.1000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.126</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.182</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.19800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.20699999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6163,6 +6633,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.7000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.13600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.158</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.16200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.185</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.19400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.19800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.20599999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6510,38 +7040,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6594,6 +7092,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>48</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>2</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -7277,6 +7813,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.4000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.193</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.219</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.249</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.254</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.28899989999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.29899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.307</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.311</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7384,6 +7980,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.189</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.20399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.20599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.214</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.23400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.24199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.254</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.28100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.28499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.29799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.30499999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7731,38 +8387,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -7815,6 +8439,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>48</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>3</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -8498,6 +9160,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>7.3999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.126</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.156</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.224</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.254</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.28299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.30499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.307</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.313</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.315</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8605,6 +9327,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.106</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.151</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.191</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.24099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.253</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.29099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.29799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.30199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.316</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8952,38 +9734,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -9036,6 +9786,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>48</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>5</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -9719,6 +10507,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.183</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.249</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.27900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.28499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.29199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.30299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.315</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.31900000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9826,6 +10674,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.8000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.186</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.216</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.24299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.251</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.27300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.28699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.29899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.30499989999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.3119999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10173,38 +11081,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -10257,6 +11133,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>96</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>2</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -10940,6 +11854,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.114</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.41299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.42399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.436</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.44600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.46</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11047,6 +12021,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>8.6999999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.156</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.223</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.248</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.32600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.35399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.36599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.38200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.39400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.40500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.41799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.42899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.437</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11394,38 +12428,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -11478,6 +12480,44 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>Display </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>96</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="sk-SK" sz="2400"/>
+              <a:t>, MLES depth </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>3</a:t>
+            </a:r>
+            <a:endParaRPr lang="sk-SK" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -12161,6 +13201,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.222</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.249</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.32300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.36799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.379</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.39200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.40100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.41599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.44900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.45600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.46700000000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -12268,6 +13368,66 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.108</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.224</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26900000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.28599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.30599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.36199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.376</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.39200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.39700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.40500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.42099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.42899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.434</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.441</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -12615,38 +13775,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="sk-SK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -19512,8 +20640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -19573,6 +20701,12 @@
       <c r="C5">
         <v>0.129</v>
       </c>
+      <c r="F5">
+        <v>0.114</v>
+      </c>
+      <c r="G5">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -19584,6 +20718,12 @@
       <c r="C6">
         <v>0.33</v>
       </c>
+      <c r="F6">
+        <v>0.192</v>
+      </c>
+      <c r="G6">
+        <v>0.17</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -19595,6 +20735,12 @@
       <c r="C7">
         <v>0.495</v>
       </c>
+      <c r="F7">
+        <v>0.245</v>
+      </c>
+      <c r="G7">
+        <v>0.219</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -19606,6 +20752,12 @@
       <c r="C8">
         <v>0.60699999999999998</v>
       </c>
+      <c r="F8">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.253</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -19617,6 +20769,12 @@
       <c r="C9">
         <v>0.65700000000000003</v>
       </c>
+      <c r="F9">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G9">
+        <v>0.27300000000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -19628,6 +20786,12 @@
       <c r="C10">
         <v>0.70399999999999996</v>
       </c>
+      <c r="F10">
+        <v>0.318</v>
+      </c>
+      <c r="G10">
+        <v>0.29499999999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -19639,6 +20803,12 @@
       <c r="C11">
         <v>0.72599999999999998</v>
       </c>
+      <c r="F11">
+        <v>0.33</v>
+      </c>
+      <c r="G11">
+        <v>0.312</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -19650,6 +20820,12 @@
       <c r="C12">
         <v>0.74</v>
       </c>
+      <c r="F12">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.32900000000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -19661,6 +20837,12 @@
       <c r="C13">
         <v>0.752</v>
       </c>
+      <c r="F13">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="G13">
+        <v>0.34499999999999997</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -19672,6 +20854,12 @@
       <c r="C14">
         <v>0.75900009999999996</v>
       </c>
+      <c r="F14">
+        <v>0.373</v>
+      </c>
+      <c r="G14">
+        <v>0.36199999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -19683,6 +20871,12 @@
       <c r="C15">
         <v>0.76700009999999996</v>
       </c>
+      <c r="F15">
+        <v>0.39</v>
+      </c>
+      <c r="G15">
+        <v>0.36799999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -19694,8 +20888,14 @@
       <c r="C16">
         <v>0.77400009999999997</v>
       </c>
+      <c r="F16">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="G16">
+        <v>0.377</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -19705,8 +20905,14 @@
       <c r="C17">
         <v>0.78200009999999998</v>
       </c>
+      <c r="F17">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.38900000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -19716,8 +20922,14 @@
       <c r="C18">
         <v>0.79600009999999999</v>
       </c>
+      <c r="F18">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.39900000000000002</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -19727,8 +20939,14 @@
       <c r="C19">
         <v>0.8050001</v>
       </c>
+      <c r="F19">
+        <v>0.43</v>
+      </c>
+      <c r="G19">
+        <v>0.41099999999999998</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -19738,8 +20956,14 @@
       <c r="C20">
         <v>0.8140001</v>
       </c>
+      <c r="F20">
+        <v>0.442</v>
+      </c>
+      <c r="G20">
+        <v>0.42</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -19749,8 +20973,14 @@
       <c r="C21">
         <v>0.82300010000000001</v>
       </c>
+      <c r="F21">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="G21">
+        <v>0.43</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -19760,8 +20990,14 @@
       <c r="C22">
         <v>0.83000019999999997</v>
       </c>
+      <c r="F22">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="G22">
+        <v>0.44400000000000001</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -19771,8 +21007,14 @@
       <c r="C23">
         <v>0.83500019999999997</v>
       </c>
+      <c r="F23">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="G23">
+        <v>0.44900000000000001</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -19781,6 +21023,12 @@
       </c>
       <c r="C24">
         <v>0.84600010000000003</v>
+      </c>
+      <c r="F24">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="G24">
+        <v>0.45700000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -19793,8 +21041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -19854,6 +21102,12 @@
       <c r="C5">
         <v>0.11600000000000001</v>
       </c>
+      <c r="F5">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G5">
+        <v>3.3000000000000002E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -19865,6 +21119,12 @@
       <c r="C6">
         <v>0.2</v>
       </c>
+      <c r="F6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>5.2999999999999999E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -19876,6 +21136,12 @@
       <c r="C7">
         <v>0.27100000000000002</v>
       </c>
+      <c r="F7">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G7">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -19887,6 +21153,12 @@
       <c r="C8">
         <v>0.32900000000000001</v>
       </c>
+      <c r="F8">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="G8">
+        <v>8.6999999999999994E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -19898,6 +21170,12 @@
       <c r="C9">
         <v>0.36799999999999999</v>
       </c>
+      <c r="F9">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="G9">
+        <v>9.4E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -19909,6 +21187,12 @@
       <c r="C10">
         <v>0.40899999999999997</v>
       </c>
+      <c r="F10">
+        <v>0.113</v>
+      </c>
+      <c r="G10">
+        <v>0.10199999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -19920,6 +21204,12 @@
       <c r="C11">
         <v>0.43099999999999999</v>
       </c>
+      <c r="F11">
+        <v>0.121</v>
+      </c>
+      <c r="G11">
+        <v>0.115</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -19931,6 +21221,12 @@
       <c r="C12">
         <v>0.45300000000000001</v>
       </c>
+      <c r="F12">
+        <v>0.125</v>
+      </c>
+      <c r="G12">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -19942,6 +21238,12 @@
       <c r="C13">
         <v>0.46899999999999997</v>
       </c>
+      <c r="F13">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.13200000000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -19953,6 +21255,12 @@
       <c r="C14">
         <v>0.48</v>
       </c>
+      <c r="F14">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.13600000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -19964,6 +21272,12 @@
       <c r="C15">
         <v>0.49099999999999999</v>
       </c>
+      <c r="F15">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.14199999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -19975,8 +21289,14 @@
       <c r="C16">
         <v>0.504</v>
       </c>
+      <c r="F16">
+        <v>0.159</v>
+      </c>
+      <c r="G16">
+        <v>0.15</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -19986,8 +21306,14 @@
       <c r="C17">
         <v>0.51500000000000001</v>
       </c>
+      <c r="F17">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.158</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -19997,8 +21323,14 @@
       <c r="C18">
         <v>0.52</v>
       </c>
+      <c r="F18">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.16900000000000001</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -20008,8 +21340,14 @@
       <c r="C19">
         <v>0.52800000000000002</v>
       </c>
+      <c r="F19">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G19">
+        <v>0.17399999999999999</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -20019,8 +21357,14 @@
       <c r="C20">
         <v>0.53</v>
       </c>
+      <c r="F20">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.17699999999999999</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -20030,8 +21374,14 @@
       <c r="C21">
         <v>0.53100000000000003</v>
       </c>
+      <c r="F21">
+        <v>0.191</v>
+      </c>
+      <c r="G21">
+        <v>0.184</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -20041,8 +21391,14 @@
       <c r="C22">
         <v>0.53199989999999997</v>
       </c>
+      <c r="F22">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.19500000000000001</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -20052,8 +21408,14 @@
       <c r="C23">
         <v>0.53500000000000003</v>
       </c>
+      <c r="F23">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -20062,6 +21424,12 @@
       </c>
       <c r="C24">
         <v>0.53600000000000003</v>
+      </c>
+      <c r="F24">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.20499999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -20074,8 +21442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -20135,6 +21503,12 @@
       <c r="C5">
         <v>0.13300000000000001</v>
       </c>
+      <c r="F5">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="G5">
+        <v>3.6999999999999998E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -20146,6 +21520,12 @@
       <c r="C6">
         <v>0.26700000000000002</v>
       </c>
+      <c r="F6">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -20157,6 +21537,12 @@
       <c r="C7">
         <v>0.34899999999999998</v>
       </c>
+      <c r="F7">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="G7">
+        <v>7.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -20168,6 +21554,12 @@
       <c r="C8">
         <v>0.41899999999999998</v>
       </c>
+      <c r="F8">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="G8">
+        <v>9.2999999999999999E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -20179,6 +21571,12 @@
       <c r="C9">
         <v>0.47</v>
       </c>
+      <c r="F9">
+        <v>0.11</v>
+      </c>
+      <c r="G9">
+        <v>0.107</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -20190,6 +21588,12 @@
       <c r="C10">
         <v>0.51000009999999996</v>
       </c>
+      <c r="F10">
+        <v>0.127</v>
+      </c>
+      <c r="G10">
+        <v>0.11799999999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -20201,6 +21605,12 @@
       <c r="C11">
         <v>0.53400000000000003</v>
       </c>
+      <c r="F11">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.13100000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -20212,6 +21622,12 @@
       <c r="C12">
         <v>0.56100000000000005</v>
       </c>
+      <c r="F12">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.13800000000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -20223,6 +21639,12 @@
       <c r="C13">
         <v>0.57900010000000002</v>
       </c>
+      <c r="F13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="G13">
+        <v>0.14899999999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -20234,6 +21656,12 @@
       <c r="C14">
         <v>0.58600010000000002</v>
       </c>
+      <c r="F14">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.152</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -20245,6 +21673,12 @@
       <c r="C15">
         <v>0.59800010000000003</v>
       </c>
+      <c r="F15">
+        <v>0.155</v>
+      </c>
+      <c r="G15">
+        <v>0.157</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -20256,8 +21690,14 @@
       <c r="C16">
         <v>0.60800010000000004</v>
       </c>
+      <c r="F16">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="G16">
+        <v>0.16300000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -20267,8 +21707,14 @@
       <c r="C17">
         <v>0.61500010000000005</v>
       </c>
+      <c r="F17">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.16900000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -20278,8 +21724,14 @@
       <c r="C18">
         <v>0.62300009999999995</v>
       </c>
+      <c r="F18">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.17699999999999999</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -20289,8 +21741,14 @@
       <c r="C19">
         <v>0.63400009999999996</v>
       </c>
+      <c r="F19">
+        <v>0.186</v>
+      </c>
+      <c r="G19">
+        <v>0.186</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -20300,8 +21758,14 @@
       <c r="C20">
         <v>0.63600009999999996</v>
       </c>
+      <c r="F20">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.19</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -20311,8 +21775,14 @@
       <c r="C21">
         <v>0.64000009999999996</v>
       </c>
+      <c r="F21">
+        <v>0.2</v>
+      </c>
+      <c r="G21">
+        <v>0.19500000000000001</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -20322,8 +21792,14 @@
       <c r="C22">
         <v>0.64400009999999996</v>
       </c>
+      <c r="F22">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="G22">
+        <v>0.20599999999999999</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -20333,8 +21809,14 @@
       <c r="C23">
         <v>0.64700009999999997</v>
       </c>
+      <c r="F23">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="G23">
+        <v>0.21199999999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -20343,6 +21825,12 @@
       </c>
       <c r="C24">
         <v>0.65000020000000003</v>
+      </c>
+      <c r="F24">
+        <v>0.217</v>
+      </c>
+      <c r="G24">
+        <v>0.214</v>
       </c>
     </row>
   </sheetData>
@@ -20355,8 +21843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -20416,6 +21904,12 @@
       <c r="C5">
         <v>7.1999999999999995E-2</v>
       </c>
+      <c r="F5">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="G5">
+        <v>3.7999999999999999E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -20427,6 +21921,12 @@
       <c r="C6">
         <v>0.19900000000000001</v>
       </c>
+      <c r="F6">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G6">
+        <v>6.7000000000000004E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -20438,6 +21938,12 @@
       <c r="C7">
         <v>0.33</v>
       </c>
+      <c r="F7">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G7">
+        <v>7.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -20449,6 +21955,12 @@
       <c r="C8">
         <v>0.44700000000000001</v>
       </c>
+      <c r="F8">
+        <v>0.109</v>
+      </c>
+      <c r="G8">
+        <v>0.10100000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -20460,6 +21972,12 @@
       <c r="C9">
         <v>0.51600000000000001</v>
       </c>
+      <c r="F9">
+        <v>0.126</v>
+      </c>
+      <c r="G9">
+        <v>0.111</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -20471,6 +21989,12 @@
       <c r="C10">
         <v>0.5689999</v>
       </c>
+      <c r="F10">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -20482,6 +22006,12 @@
       <c r="C11">
         <v>0.61</v>
       </c>
+      <c r="F11">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.13600000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -20493,6 +22023,12 @@
       <c r="C12">
         <v>0.627</v>
       </c>
+      <c r="F12">
+        <v>0.15</v>
+      </c>
+      <c r="G12">
+        <v>0.14499999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -20504,6 +22040,12 @@
       <c r="C13">
         <v>0.65</v>
       </c>
+      <c r="F13">
+        <v>0.154</v>
+      </c>
+      <c r="G13">
+        <v>0.153</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -20515,6 +22057,12 @@
       <c r="C14">
         <v>0.67</v>
       </c>
+      <c r="F14">
+        <v>0.158</v>
+      </c>
+      <c r="G14">
+        <v>0.153</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -20526,6 +22074,12 @@
       <c r="C15">
         <v>0.67999989999999999</v>
       </c>
+      <c r="F15">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.158</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -20537,8 +22091,14 @@
       <c r="C16">
         <v>0.6859999</v>
       </c>
+      <c r="F16">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.16200000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -20548,8 +22108,14 @@
       <c r="C17">
         <v>0.6899999</v>
       </c>
+      <c r="F17">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="G17">
+        <v>0.16700000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -20559,8 +22125,14 @@
       <c r="C18">
         <v>0.69699999999999995</v>
       </c>
+      <c r="F18">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.17799999999999999</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -20570,8 +22142,14 @@
       <c r="C19">
         <v>0.70299990000000001</v>
       </c>
+      <c r="F19">
+        <v>0.182</v>
+      </c>
+      <c r="G19">
+        <v>0.185</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -20581,8 +22159,14 @@
       <c r="C20">
         <v>0.70799990000000002</v>
       </c>
+      <c r="F20">
+        <v>0.19</v>
+      </c>
+      <c r="G20">
+        <v>0.19</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -20592,8 +22176,14 @@
       <c r="C21">
         <v>0.71299990000000002</v>
       </c>
+      <c r="F21">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="G21">
+        <v>0.19400000000000001</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -20603,8 +22193,14 @@
       <c r="C22">
         <v>0.71599999999999997</v>
       </c>
+      <c r="F22">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.19800000000000001</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -20614,8 +22210,14 @@
       <c r="C23">
         <v>0.72</v>
       </c>
+      <c r="F23">
+        <v>0.20599999999999999</v>
+      </c>
+      <c r="G23">
+        <v>0.20200000000000001</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -20624,6 +22226,12 @@
       </c>
       <c r="C24">
         <v>0.72499999999999998</v>
+      </c>
+      <c r="F24">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="G24">
+        <v>0.20599999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -20636,8 +22244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -20697,6 +22305,12 @@
       <c r="C5">
         <v>0.128</v>
       </c>
+      <c r="F5">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>6.9000000000000006E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -20708,6 +22322,12 @@
       <c r="C6">
         <v>0.216</v>
       </c>
+      <c r="F6">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.10199999999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -20719,6 +22339,12 @@
       <c r="C7">
         <v>0.28699999999999998</v>
       </c>
+      <c r="F7">
+        <v>0.125</v>
+      </c>
+      <c r="G7">
+        <v>0.124</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -20730,6 +22356,12 @@
       <c r="C8">
         <v>0.33800000000000002</v>
       </c>
+      <c r="F8">
+        <v>0.152</v>
+      </c>
+      <c r="G8">
+        <v>0.14299999999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -20741,6 +22373,12 @@
       <c r="C9">
         <v>0.372</v>
       </c>
+      <c r="F9">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.16800000000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -20752,6 +22390,12 @@
       <c r="C10">
         <v>0.39800000000000002</v>
       </c>
+      <c r="F10">
+        <v>0.182</v>
+      </c>
+      <c r="G10">
+        <v>0.189</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -20763,6 +22407,12 @@
       <c r="C11">
         <v>0.41499999999999998</v>
       </c>
+      <c r="F11">
+        <v>0.193</v>
+      </c>
+      <c r="G11">
+        <v>0.20399999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -20774,6 +22424,12 @@
       <c r="C12">
         <v>0.433</v>
       </c>
+      <c r="F12">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.20599999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -20785,6 +22441,12 @@
       <c r="C13">
         <v>0.439</v>
       </c>
+      <c r="F13">
+        <v>0.219</v>
+      </c>
+      <c r="G13">
+        <v>0.214</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -20796,6 +22458,12 @@
       <c r="C14">
         <v>0.45</v>
       </c>
+      <c r="F14">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="G14">
+        <v>0.22800000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -20807,6 +22475,12 @@
       <c r="C15">
         <v>0.45400000000000001</v>
       </c>
+      <c r="F15">
+        <v>0.249</v>
+      </c>
+      <c r="G15">
+        <v>0.23400000000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -20818,8 +22492,14 @@
       <c r="C16">
         <v>0.46300000000000002</v>
       </c>
+      <c r="F16">
+        <v>0.254</v>
+      </c>
+      <c r="G16">
+        <v>0.24199999999999999</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -20829,8 +22509,14 @@
       <c r="C17">
         <v>0.47199999999999998</v>
       </c>
+      <c r="F17">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.254</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -20840,8 +22526,14 @@
       <c r="C18">
         <v>0.47699999999999998</v>
       </c>
+      <c r="F18">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.26200000000000001</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -20851,8 +22543,14 @@
       <c r="C19">
         <v>0.48299999999999998</v>
       </c>
+      <c r="F19">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="G19">
+        <v>0.27500000000000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -20862,8 +22560,14 @@
       <c r="C20">
         <v>0.48499999999999999</v>
       </c>
+      <c r="F20">
+        <v>0.28899989999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.28100000000000003</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -20873,8 +22577,14 @@
       <c r="C21">
         <v>0.49</v>
       </c>
+      <c r="F21">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G21">
+        <v>0.28499999999999998</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -20884,8 +22594,14 @@
       <c r="C22">
         <v>0.49399999999999999</v>
       </c>
+      <c r="F22">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="G22">
+        <v>0.28999999999999998</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -20895,8 +22611,14 @@
       <c r="C23">
         <v>0.497</v>
       </c>
+      <c r="F23">
+        <v>0.307</v>
+      </c>
+      <c r="G23">
+        <v>0.29799999999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -20905,6 +22627,12 @@
       </c>
       <c r="C24">
         <v>0.497</v>
+      </c>
+      <c r="F24">
+        <v>0.311</v>
+      </c>
+      <c r="G24">
+        <v>0.30499999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -20917,8 +22645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -20978,6 +22706,12 @@
       <c r="C5">
         <v>0.16400000000000001</v>
       </c>
+      <c r="F5">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="G5">
+        <v>6.3E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -20989,6 +22723,12 @@
       <c r="C6">
         <v>0.31</v>
       </c>
+      <c r="F6">
+        <v>0.126</v>
+      </c>
+      <c r="G6">
+        <v>0.106</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -21000,6 +22740,12 @@
       <c r="C7">
         <v>0.4</v>
       </c>
+      <c r="F7">
+        <v>0.156</v>
+      </c>
+      <c r="G7">
+        <v>0.13700000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -21011,6 +22757,12 @@
       <c r="C8">
         <v>0.46200000000000002</v>
       </c>
+      <c r="F8">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.151</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -21022,6 +22774,12 @@
       <c r="C9">
         <v>0.50700000000000001</v>
       </c>
+      <c r="F9">
+        <v>0.19</v>
+      </c>
+      <c r="G9">
+        <v>0.17599999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -21033,6 +22791,12 @@
       <c r="C10">
         <v>0.53400000000000003</v>
       </c>
+      <c r="F10">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.191</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -21044,6 +22808,12 @@
       <c r="C11">
         <v>0.56399999999999995</v>
       </c>
+      <c r="F11">
+        <v>0.22</v>
+      </c>
+      <c r="G11">
+        <v>0.20499999999999999</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -21055,6 +22825,12 @@
       <c r="C12">
         <v>0.57499999999999996</v>
       </c>
+      <c r="F12">
+        <v>0.224</v>
+      </c>
+      <c r="G12">
+        <v>0.21299999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -21066,6 +22842,12 @@
       <c r="C13">
         <v>0.58599999999999997</v>
       </c>
+      <c r="F13">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.22800000000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -21077,6 +22859,12 @@
       <c r="C14">
         <v>0.60499999999999998</v>
       </c>
+      <c r="F14">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.23699999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -21088,6 +22876,12 @@
       <c r="C15">
         <v>0.61499990000000004</v>
       </c>
+      <c r="F15">
+        <v>0.254</v>
+      </c>
+      <c r="G15">
+        <v>0.24099999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -21099,8 +22893,14 @@
       <c r="C16">
         <v>0.62599990000000005</v>
       </c>
+      <c r="F16">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="G16">
+        <v>0.253</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -21110,8 +22910,14 @@
       <c r="C17">
         <v>0.63199989999999995</v>
       </c>
+      <c r="F17">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G17">
+        <v>0.26500000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -21121,8 +22927,14 @@
       <c r="C18">
         <v>0.63699989999999995</v>
       </c>
+      <c r="F18">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G18">
+        <v>0.27400000000000002</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -21132,8 +22944,14 @@
       <c r="C19">
         <v>0.64299989999999996</v>
       </c>
+      <c r="F19">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.28399999999999997</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -21143,8 +22961,14 @@
       <c r="C20">
         <v>0.64799989999999996</v>
       </c>
+      <c r="F20">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.29099999999999998</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -21154,8 +22978,14 @@
       <c r="C21">
         <v>0.65199989999999997</v>
       </c>
+      <c r="F21">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0.29799999999999999</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -21165,8 +22995,14 @@
       <c r="C22">
         <v>0.65299989999999997</v>
       </c>
+      <c r="F22">
+        <v>0.307</v>
+      </c>
+      <c r="G22">
+        <v>0.30199999999999999</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -21176,8 +23012,14 @@
       <c r="C23">
         <v>0.65499989999999997</v>
       </c>
+      <c r="F23">
+        <v>0.313</v>
+      </c>
+      <c r="G23">
+        <v>0.312</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -21186,6 +23028,12 @@
       </c>
       <c r="C24">
         <v>0.65699980000000002</v>
+      </c>
+      <c r="F24">
+        <v>0.315</v>
+      </c>
+      <c r="G24">
+        <v>0.316</v>
       </c>
     </row>
   </sheetData>
@@ -21198,8 +23046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21259,6 +23107,12 @@
       <c r="C5">
         <v>9.0999999999999998E-2</v>
       </c>
+      <c r="F5">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -21270,6 +23124,12 @@
       <c r="C6">
         <v>0.23699999999999999</v>
       </c>
+      <c r="F6">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="G6">
+        <v>9.8000000000000004E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -21281,6 +23141,12 @@
       <c r="C7">
         <v>0.40699999999999997</v>
       </c>
+      <c r="F7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.13600000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -21292,6 +23158,12 @@
       <c r="C8">
         <v>0.51500000000000001</v>
       </c>
+      <c r="F8">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.16200000000000001</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -21303,6 +23175,12 @@
       <c r="C9">
         <v>0.57099999999999995</v>
       </c>
+      <c r="F9">
+        <v>0.183</v>
+      </c>
+      <c r="G9">
+        <v>0.186</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -21314,6 +23192,12 @@
       <c r="C10">
         <v>0.61199999999999999</v>
       </c>
+      <c r="F10">
+        <v>0.21</v>
+      </c>
+      <c r="G10">
+        <v>0.19500000000000001</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -21325,6 +23209,12 @@
       <c r="C11">
         <v>0.65200000000000002</v>
       </c>
+      <c r="F11">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="G11">
+        <v>0.20200000000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -21336,6 +23226,12 @@
       <c r="C12">
         <v>0.67600000000000005</v>
       </c>
+      <c r="F12">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.216</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -21347,6 +23243,12 @@
       <c r="C13">
         <v>0.69099999999999995</v>
       </c>
+      <c r="F13">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="G13">
+        <v>0.23699999999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -21358,6 +23260,12 @@
       <c r="C14">
         <v>0.70099999999999996</v>
       </c>
+      <c r="F14">
+        <v>0.249</v>
+      </c>
+      <c r="G14">
+        <v>0.24299999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -21369,6 +23277,12 @@
       <c r="C15">
         <v>0.71299999999999997</v>
       </c>
+      <c r="F15">
+        <v>0.26</v>
+      </c>
+      <c r="G15">
+        <v>0.251</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -21380,8 +23294,14 @@
       <c r="C16">
         <v>0.72099999999999997</v>
       </c>
+      <c r="F16">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="G16">
+        <v>0.25900000000000001</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -21391,8 +23311,14 @@
       <c r="C17">
         <v>0.72899999999999998</v>
       </c>
+      <c r="F17">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G17">
+        <v>0.26500000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -21402,8 +23328,14 @@
       <c r="C18">
         <v>0.73200010000000004</v>
       </c>
+      <c r="F18">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="G18">
+        <v>0.27300000000000002</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -21413,8 +23345,14 @@
       <c r="C19">
         <v>0.74000010000000005</v>
       </c>
+      <c r="F19">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.27900000000000003</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -21424,8 +23362,14 @@
       <c r="C20">
         <v>0.74400010000000005</v>
       </c>
+      <c r="F20">
+        <v>0.3</v>
+      </c>
+      <c r="G20">
+        <v>0.28699999999999998</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -21435,8 +23379,14 @@
       <c r="C21">
         <v>0.75200009999999995</v>
       </c>
+      <c r="F21">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0.29899999999999999</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -21446,8 +23396,14 @@
       <c r="C22">
         <v>0.75500009999999995</v>
       </c>
+      <c r="F22">
+        <v>0.312</v>
+      </c>
+      <c r="G22">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -21457,8 +23413,14 @@
       <c r="C23">
         <v>0.76100009999999996</v>
       </c>
+      <c r="F23">
+        <v>0.315</v>
+      </c>
+      <c r="G23">
+        <v>0.30499989999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -21467,6 +23429,12 @@
       </c>
       <c r="C24">
         <v>0.76500009999999996</v>
+      </c>
+      <c r="F24">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="G24">
+        <v>0.3119999</v>
       </c>
     </row>
   </sheetData>
@@ -21479,8 +23447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21540,6 +23508,12 @@
       <c r="C5">
         <v>0.156</v>
       </c>
+      <c r="F5">
+        <v>0.114</v>
+      </c>
+      <c r="G5">
+        <v>8.6999999999999994E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -21551,6 +23525,12 @@
       <c r="C6">
         <v>0.23200000000000001</v>
       </c>
+      <c r="F6">
+        <v>0.156</v>
+      </c>
+      <c r="G6">
+        <v>0.13100000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -21562,6 +23542,12 @@
       <c r="C7">
         <v>0.28599999999999998</v>
       </c>
+      <c r="F7">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.156</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -21573,6 +23559,12 @@
       <c r="C8">
         <v>0.33</v>
       </c>
+      <c r="F8">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.185</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -21584,6 +23576,12 @@
       <c r="C9">
         <v>0.35299999999999998</v>
       </c>
+      <c r="F9">
+        <v>0.25</v>
+      </c>
+      <c r="G9">
+        <v>0.223</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -21595,6 +23593,12 @@
       <c r="C10">
         <v>0.375</v>
       </c>
+      <c r="F10">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.248</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -21606,6 +23610,12 @@
       <c r="C11">
         <v>0.40100000000000002</v>
       </c>
+      <c r="F11">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -21617,6 +23627,12 @@
       <c r="C12">
         <v>0.41799999999999998</v>
       </c>
+      <c r="F12">
+        <v>0.312</v>
+      </c>
+      <c r="G12">
+        <v>0.29499999999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -21628,6 +23644,12 @@
       <c r="C13">
         <v>0.442</v>
       </c>
+      <c r="F13">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.312</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -21639,6 +23661,12 @@
       <c r="C14">
         <v>0.47399999999999998</v>
       </c>
+      <c r="F14">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="G14">
+        <v>0.32600000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -21650,6 +23678,12 @@
       <c r="C15">
         <v>0.50399989999999995</v>
       </c>
+      <c r="F15">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="G15">
+        <v>0.33800000000000002</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -21661,8 +23695,14 @@
       <c r="C16">
         <v>0.53500000000000003</v>
       </c>
+      <c r="F16">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.35399999999999998</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -21672,8 +23712,14 @@
       <c r="C17">
         <v>0.5649999</v>
       </c>
+      <c r="F17">
+        <v>0.38</v>
+      </c>
+      <c r="G17">
+        <v>0.36599999999999999</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -21683,8 +23729,14 @@
       <c r="C18">
         <v>0.59899990000000003</v>
       </c>
+      <c r="F18">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.38200000000000001</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -21694,8 +23746,14 @@
       <c r="C19">
         <v>0.62499990000000005</v>
       </c>
+      <c r="F19">
+        <v>0.4</v>
+      </c>
+      <c r="G19">
+        <v>0.39400000000000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -21705,8 +23763,14 @@
       <c r="C20">
         <v>0.65200000000000002</v>
       </c>
+      <c r="F20">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="G20">
+        <v>0.40500000000000003</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -21716,8 +23780,14 @@
       <c r="C21">
         <v>0.67400000000000004</v>
       </c>
+      <c r="F21">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0.41</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -21727,8 +23797,14 @@
       <c r="C22">
         <v>0.69499999999999995</v>
       </c>
+      <c r="F22">
+        <v>0.436</v>
+      </c>
+      <c r="G22">
+        <v>0.41799999999999998</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -21738,8 +23814,14 @@
       <c r="C23">
         <v>0.71499999999999997</v>
       </c>
+      <c r="F23">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.42899999999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -21748,6 +23830,12 @@
       </c>
       <c r="C24">
         <v>0.73</v>
+      </c>
+      <c r="F24">
+        <v>0.46</v>
+      </c>
+      <c r="G24">
+        <v>0.437</v>
       </c>
     </row>
   </sheetData>
@@ -21760,8 +23848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -21821,6 +23909,12 @@
       <c r="C5">
         <v>0.187</v>
       </c>
+      <c r="F5">
+        <v>0.122</v>
+      </c>
+      <c r="G5">
+        <v>0.108</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -21832,6 +23926,12 @@
       <c r="C6">
         <v>0.36899999999999999</v>
       </c>
+      <c r="F6">
+        <v>0.19</v>
+      </c>
+      <c r="G6">
+        <v>0.16400000000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -21843,6 +23943,12 @@
       <c r="C7">
         <v>0.46899999999999997</v>
       </c>
+      <c r="F7">
+        <v>0.222</v>
+      </c>
+      <c r="G7">
+        <v>0.19900000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -21854,6 +23960,12 @@
       <c r="C8">
         <v>0.52800000000000002</v>
       </c>
+      <c r="F8">
+        <v>0.249</v>
+      </c>
+      <c r="G8">
+        <v>0.224</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -21865,6 +23977,12 @@
       <c r="C9">
         <v>0.55600000000000005</v>
       </c>
+      <c r="F9">
+        <v>0.27</v>
+      </c>
+      <c r="G9">
+        <v>0.23899999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -21876,6 +23994,12 @@
       <c r="C10">
         <v>0.58199999999999996</v>
       </c>
+      <c r="F10">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="G10">
+        <v>0.26900000000000002</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -21887,6 +24011,12 @@
       <c r="C11">
         <v>0.59899999999999998</v>
       </c>
+      <c r="F11">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.28599999999999998</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -21898,6 +24028,12 @@
       <c r="C12">
         <v>0.61199999999999999</v>
       </c>
+      <c r="F12">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.30599999999999999</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -21909,6 +24045,12 @@
       <c r="C13">
         <v>0.62500009999999995</v>
       </c>
+      <c r="F13">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="G13">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -21920,6 +24062,12 @@
       <c r="C14">
         <v>0.63600000000000001</v>
       </c>
+      <c r="F14">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="G14">
+        <v>0.33300000000000002</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -21931,6 +24079,12 @@
       <c r="C15">
         <v>0.64600000000000002</v>
       </c>
+      <c r="F15">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -21942,8 +24096,14 @@
       <c r="C16">
         <v>0.66100000000000003</v>
       </c>
+      <c r="F16">
+        <v>0.379</v>
+      </c>
+      <c r="G16">
+        <v>0.36199999999999999</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>13</v>
       </c>
@@ -21953,8 +24113,14 @@
       <c r="C17">
         <v>0.67500000000000004</v>
       </c>
+      <c r="F17">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="G17">
+        <v>0.376</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>14</v>
       </c>
@@ -21964,8 +24130,14 @@
       <c r="C18">
         <v>0.69199999999999995</v>
       </c>
+      <c r="F18">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.39200000000000002</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>15</v>
       </c>
@@ -21975,8 +24147,14 @@
       <c r="C19">
         <v>0.70799999999999996</v>
       </c>
+      <c r="F19">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.39700000000000002</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>16</v>
       </c>
@@ -21986,8 +24164,14 @@
       <c r="C20">
         <v>0.71499999999999997</v>
       </c>
+      <c r="F20">
+        <v>0.43</v>
+      </c>
+      <c r="G20">
+        <v>0.40500000000000003</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>17</v>
       </c>
@@ -21997,8 +24181,14 @@
       <c r="C21">
         <v>0.73200010000000004</v>
       </c>
+      <c r="F21">
+        <v>0.442</v>
+      </c>
+      <c r="G21">
+        <v>0.42099999999999999</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>18</v>
       </c>
@@ -22008,8 +24198,14 @@
       <c r="C22">
         <v>0.747</v>
       </c>
+      <c r="F22">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.42899999999999999</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>19</v>
       </c>
@@ -22019,8 +24215,14 @@
       <c r="C23">
         <v>0.76000009999999996</v>
       </c>
+      <c r="F23">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="G23">
+        <v>0.434</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>20</v>
       </c>
@@ -22029,6 +24231,12 @@
       </c>
       <c r="C24">
         <v>0.77100000000000002</v>
+      </c>
+      <c r="F24">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="G24">
+        <v>0.441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>